<commit_message>
Update images in exports to bitmaps
</commit_message>
<xml_diff>
--- a/export/cdisc_biomedical_concepts_20231003.xlsx
+++ b/export/cdisc_biomedical_concepts_20231003.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_github\cdisc-org\COSMoS\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B667DB-437A-4D64-824C-575C602448D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECE4E218-9C76-44F2-94D7-6A6503D441D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="390" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4853,17 +4853,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>240603</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>18288</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>370952</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>113729</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F7D48F4-5492-D53C-67DD-82D41FFBE2DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{133164A3-64EC-EA30-BD5B-10FF323D2C29}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4880,7 +4880,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10020300" y="733425"/>
-          <a:ext cx="5574603" cy="6095238"/>
+          <a:ext cx="4180952" cy="4571429"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>

</xml_diff>